<commit_message>
textures,spirit consumable, mc wip, consumable panel
</commit_message>
<xml_diff>
--- a/Character.xlsx
+++ b/Character.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>1 + floor * 5</t>
+  </si>
+  <si>
+    <t>5 - floor *10</t>
   </si>
 </sst>
 </file>
@@ -450,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,9 +466,10 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -481,8 +485,11 @@
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -498,8 +505,11 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="7"/>
@@ -509,15 +519,18 @@
       <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="6"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="7"/>

</xml_diff>